<commit_message>
download history saved in files
</commit_message>
<xml_diff>
--- a/misc/api_endpoints.xlsx
+++ b/misc/api_endpoints.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\github\projects\benyon_sports\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A00DF38-81A0-4B71-AA3D-EA55E4073063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871A627F-5066-457F-BA10-E8FB1464A436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="api_endpoints" sheetId="1" r:id="rId1"/>
-    <sheet name="24june" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>---</t>
   </si>
@@ -104,30 +103,6 @@
   </si>
   <si>
     <t>- /</t>
-  </si>
-  <si>
-    <t>create and upload buttons appear only for admin user, not standard user</t>
-  </si>
-  <si>
-    <t>error on analytics page resolved.</t>
-  </si>
-  <si>
-    <t>When page refreshes after create user, loading spinner is now shown</t>
-  </si>
-  <si>
-    <t>search_files implemented</t>
-  </si>
-  <si>
-    <t>Document Management page: details can be viewed thru drop-down menu</t>
-  </si>
-  <si>
-    <t>an issue in backend fixed (wrong format of paths returned by search_files)</t>
-  </si>
-  <si>
-    <t>Directory structure shown to enable browsing</t>
-  </si>
-  <si>
-    <t>some extra sections removed from Document Management</t>
   </si>
 </sst>
 </file>
@@ -461,7 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -608,59 +583,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5FB2B1-9985-4130-86B9-A142ACB7D266}">
-  <dimension ref="A1:A8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>